<commit_message>
add detecção automatica da situação do motorista
</commit_message>
<xml_diff>
--- a/lista_pagamento.xlsx
+++ b/lista_pagamento.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus.lima\Desktop\scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus.lima\Desktop\scripts\script_pg_salario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2ABAC7F-708E-477B-85EF-503E31C62058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33126071-9123-4A0A-8B38-8C4F9EB98C0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{49A29A69-E823-4A0B-9244-5FA29256CC53}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>JOSE ROGERIO PEREIRA DA COSTA</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t>salario</t>
+  </si>
+  <si>
+    <t>CARLOS ALBERTO DE MENEZES</t>
+  </si>
+  <si>
+    <t>RENATO AQUINO DE PIN</t>
   </si>
 </sst>
 </file>
@@ -124,8 +130,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D349A152-E7FB-413A-8DA4-FD7664BD64D4}" name="Tabela1" displayName="Tabela1" ref="A1:C6" totalsRowShown="0">
-  <autoFilter ref="A1:C6" xr:uid="{D349A152-E7FB-413A-8DA4-FD7664BD64D4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D349A152-E7FB-413A-8DA4-FD7664BD64D4}" name="Tabela1" displayName="Tabela1" ref="A1:C8" totalsRowShown="0">
+  <autoFilter ref="A1:C8" xr:uid="{D349A152-E7FB-413A-8DA4-FD7664BD64D4}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{14B0400A-AD38-497C-B11D-A54D31564152}" name="nome"/>
     <tableColumn id="2" xr3:uid="{48F8EBA1-FB45-4C2D-AA98-AB242801D51D}" name="documento"/>
@@ -432,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{750B4FF3-ACDB-451C-A26D-65768512BB75}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,57 +463,79 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
+      <c r="A2" t="s">
+        <v>9</v>
       </c>
       <c r="B2">
-        <v>111</v>
+        <v>777</v>
       </c>
       <c r="C2">
-        <v>10</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
+      <c r="A3" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B3">
-        <v>222</v>
+        <v>666</v>
       </c>
       <c r="C3">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>333</v>
+        <v>222</v>
       </c>
       <c r="C4">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B5">
-        <v>444</v>
+        <v>111</v>
       </c>
       <c r="C5">
-        <v>40</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>333</v>
+      </c>
+      <c r="C6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>444</v>
+      </c>
+      <c r="C7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B8">
         <v>555</v>
       </c>
-      <c r="C6">
+      <c r="C8">
         <v>50</v>
       </c>
     </row>

</xml_diff>